<commit_message>
vault backup: 2023-01-19 01:25:19
</commit_message>
<xml_diff>
--- a/emotion/3.论文记录/语音情感识别-摘要-引言摘录.xlsx
+++ b/emotion/3.论文记录/语音情感识别-摘要-引言摘录.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\19115\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\3.进修\2.升学\04.硕士学习\3.研究\笔记\emotion\3.论文记录\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E547FF38-F072-4B72-87E1-E69AF57DBA94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B87F69F-EDD1-480B-A2F1-64D68D88E461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{51BD2796-7EA4-47CC-B162-5BC723D3BEC4}"/>
+    <workbookView xWindow="840" yWindow="216" windowWidth="12204" windowHeight="9816" xr2:uid="{51BD2796-7EA4-47CC-B162-5BC723D3BEC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -362,10 +363,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> 随着人工智能的不断发展，情感计算领域越来越受到研究者的关注。 情感识别是情感计算的重要组成部分，旨在从收集到的人脸、语音和文本数据中识别出有意义的信息。 在这些数据中，语音是情感信息的重要来源，它不仅包含交际内容，还包含情感等副语言信息。 近年来，语音情感识别（SER）在人工客服[1]、远程教育[2]和医学[3]等诸多领域得到了广泛的应用。 然而，由于某些特定情绪之间的严重混淆，识别语音中表达的情绪仍然具有挑战性。 特征提取是 SER 系统中的一个重要过程，旨在为不同的情绪产生有效的特征表示。 在 SER 的声学特征提取方面，基于低级描述符 (LLD) 和高级统计泛函 (HSF) [4, 5, 6] 的几个特征集，包括 INTERSPEECH-2010 [7]，GeMAPS [8]、AVEC2013 [9] 和 ComParE [10] 已被开发用于广泛的应用。 随着计算能力的提高，深度学习方法成为主流，为高级特征捕获提供了卓越的能力。 例如，Han 等人。 [11] 使用深度神经网络 (DNN) 提取 MFCC 和音调的片段级特征，其中包含情感上有效的信息。 毛等。 [12] 首先采用卷积神经网络 (CNN) 从 SER 的频谱图中学习空间特征，并在一些基准数据集上表现出出色的性能。 李等。 [13] 使用递归神经网络 (RNN) 来解释情绪言语中的长上下文效应。 陈等。 [14] 使用 LSTM 学习 SER 的长期依赖性和上下文信息。 然而，大多数先前研究中的一个共同问题是特征混淆，即来自不同情感类别的聚类可能相互重叠 [15]。 为了解决这个问题，Huang 等人。 [16] 利用 hard-positive 挖掘技术来评估三元组损失的性能。 刘等人。 [17] 通过选择硬三元组提出了一个使用三元组损失的 SER 框架，以更好地区分情感分类中的混淆。 高等。 [18] 引入了度量学习来衡量三元组输入的相似性，并鼓励模型为 SER 提取更具辨别力的特征。 然而，所有以前的方法都从根据当前网络很难的训练样本中挖掘出困难三元组，从而使经过训练的特征嵌入网络容易受到不良局部最优的影响 [19, 20]。 在本文中，我们引入了一种对抗性联合损失策略来明确地激发所学特征之间的类内紧凑性和类间可分离性，其中应用生成器和鉴别器来生成对全局优化网络非常重要的硬三元组。 SER 的另一个关键问题是如何有效地突出与情感相关的区域，因为语音中的特征对情感识别的贡献不均。 受视觉分析 [21, 22] 成功的启发，研究人员引入了时空注意力来提高 SER 系统的性能 [23, 24]。 李等。 [15] 提出了时空注意力来提取频率特征。 然而，时空注意力突出了不同特征对 SER 的贡献，而忽略了语音中的时间特征。 刘等人。 [25] 引入了自我注意机制，它捕获了时间特征的长期依赖性，并允许模型专注于情感显着特征。 因此，我们提出了将时空注意力与自我注意力相结合的级联注意力，以定位一些目标情绪区域并捕获长距离依赖。 本文的主要贡献总结如下：（1）我们提出了一个级联注意力网络（CAN）来提取有效的情感特征，其中时空注意力定位一些目标情感区域，自注意力可以补偿长距离依赖 . (2) 我们引入了一种对抗性联合损失策略来区分不同类别的相似情感嵌入，其中生成器和鉴别器用于生成硬三元组以全局优化网络，而不是仅探索当前网络的现有样本。 (3) 在基准数据集 IEMOCAP 上的实验结果表明，我们的方法在 WA 和 UA 中分别达到了 76.17% 和 72.95%。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t xml:space="preserve"> 由于其复杂性，从语音中准确识别情感是一项必要但具有挑战性的任务。 以往大多数研究中存在的一个共同问题是某些特定情绪被严重错误分类。 在本文中，我们提出了一种集成级联注意和对抗性联合损失的语音情感识别框架，旨在通过更加强调难以正确分类的情感来区分混淆。 具体来说，我们提出了一个级联注意力网络来提取有效的情感特征，其中时空注意力从输入特征中选择性地定位目标情感区域。 在这些目标区域中，带有头部融合的自注意力捕获了时间特征的长距离依赖性。 此外，还提出了一种对抗性联合损失策略，以对抗性方式通过生成的硬三元组来区分具有高相似性的情感嵌入。 在基准数据集 IEMOCAP 上的实验结果表明，我们的方法在加权精度 (WA) 和未加权精度 (UA) 方面分别比最先进的策略获得了 3.17% 和 0.39% 的绝对改进。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -413,67 +410,80 @@
     <t>除了声学信息，基于语音转录的语言特征已被证明在语音情感识别 (SER) 中很有用。 然而，由于情感标记数据的稀缺和情感语音识别的困难，该研究领域难以获得可靠的语言特征和模型。 在本文中，我们建议将自动语音识别 (ASR) 输出融合到用于联合训练 SER 的管道中。 ASR 和 SER 之间的关系尚未得到充分研究，尚不清楚 ASR 的哪些特性以及如何使 SER 受益。 通过检查各种 ASR 输出和融合方法，我们的实验表明，在联合 ASR-SER 训练中，使用分层共同注意融合方法结合 ASR 隐藏和文本输出可以最大程度地提高 SER 性能。 在 IEMOCAP 语料库上，我们的方法实现了 63.4% 的加权准确率，这接近于结合地面实况成绩单所取得的基线结果。 此外，我们还提供了对 IEMOCAP 的新词错误率分析和 Wav2vec 2.0 模型的层差分析，以更好地理解 ASR 和 SER 之间的关系。</t>
   </si>
   <si>
+    <t>语音情感识别 (SER) 对于人机交互至关重要，但由于两个主要障碍仍然是一个具有挑战性的问题：数据稀缺和不平衡。 许多 SER 数据集基本上是不平衡的，其中一类（通常是中性）的数据话语比其他类的数据话语更频繁。 此外，只有少数数据资源可用于许多现有的口头语言。 为了解决这些问题，我们利用由三元组网络引导的基于 GAN 的增强模型，以在训练数据不平衡和不足的情况下提高 SER 性能。 我们进行实验并证明：1）在高度不平衡的数据集下，我们的增强策略显着提高了 SER 性能（与基线相比 +8% 的召回率）。 2) 此外，在跨语言基准测试中，我们训练了一个具有足够源语言话语但目标语言话语很少（在我们的实验中大约 50 个）的模型，我们的增强策略为所有三种目标语言的 SER 性能带来了好处。</t>
+  </si>
+  <si>
+    <t>深度学习架构的最新发展促使我们使用频谱图或音频功能（例如 MFCC），而不是手工制作的 LLD。 [6] 直接从语音频谱图中提取特征，而不是使用传统的手工制作的特征来更好地表示情感。 这些提取的特征用作卷积神经网络 (CNN) 的输入。 [7] 将 Mel 频谱图和 MFCC 用于包含两个独立神经网络的双层模型。 他们通过提取两个具有不同窗口大小的不同 Mel 频谱图来解决时频权衡问题。 此外，他们还通过实验表明，梅尔频谱图比 MFCC 更难学习。 我们目前的工作使用 MFCC。 目前，几乎所有的深度学习应用都在使用注意力机制。 注意机制可以通过更多地关注特征空间的关键区域来提高性能。 注意力还可以在一定程度上缓解黑盒问题，这是深度学习模型结构的一个缺点。 在语音识别领域，注意力机制已被用于 ASR [17, 18] 和 SER [19, 20, 21] 等任务。 特别是，在 [13] 在机器翻译任务中表现出强大的自注意力之后，自注意力也试图在 SER 任务 [6, 22] 中为关键区域分配更多权重，并证明了其有效性。 [6] 使用自我注意机制来关注出现在特定部分而不是整个话语中的情绪。 [22] 结合扩张残差网络 (DRN) 和多头自注意力来增强情绪显着信息的导入，我们在本文中将该模型表示为 DRN-MHSA。 SER 中其他最先进的模型如下。 Audio-BRE [23] 使用基于使用 MFCC 的长短期记忆 (LSTM) 的双向循环编码器 (BRE) 模型。 A-DCNN [24] 使用 SincNet 过滤器层 [25] 从语音音频中学习自定义过滤器组。 与 [6, 22] 使用现有的自注意力不同，我们提出了使用 FA 和 CA 机制改进的自注意力，并验证了检测最大振幅和学习表达表示可以提高情绪识别性能的假设。</t>
+  </si>
+  <si>
+    <t>注意力已经成为深度学习方法中最常用的机制之一。 注意机制可以帮助系统更多地关注特征空间的关键区域。 例如，高振幅区域可以在语音情感识别 (SER) 中发挥重要作用。 在本文中，我们确定了现有多头自注意力中注意力与信号幅度之间的错位。 为了改善注意力区域，我们建议结合多头自注意力使用焦点-注意力 (FA) 机制和新颖的校准-注意力 (CA) 机制。 通过FA机制，网络可以检测出片段中最大幅度的部分。 通过采用 CA 机制，网络可以通过为每个注意力头分配不同的权重来调节信息流，并提高周围上下文的利用率。 为了评估所提出的方法，使用 IEMOCAP 和 RAVDESS 数据集进行了实验。 实验结果表明，所提出的框架在两个数据集上都明显优于最先进的方法。</t>
+  </si>
+  <si>
+    <t>在本文中，我们提出了一种基于对抗性自动编码器的分类器，它可以规范潜在表示的分布以平滑类别之间的边界。 此外，我们采用多实例学习，将语音分成多个片段，以捕捉表达情绪的最显着时刻。 所提出的模型在 IEMOCAP 数据集上进行了训练，并在语料库验证集 (IEMOCAP) 和跨语料库验证集 (MELD) 上进行了评估。 实验结果表明，我们的模型优于语料库内验证的基线，并通过正则化提高了跨语料库验证的分数。</t>
+  </si>
+  <si>
+    <t>随着语音情感识别（SER）的发展，目前的研究大多是话语级的，不能适应实际场景的需要。 在本文中，我们提出了一种新颖的策略，专注于捕获对话级别的上下文信息。 基于卷积神经网络 (CNN) 和双向长短期记忆网络 (BLSTM) 学习的话语级表示，所提出的对话级方法由两个模块组成。 第一个模块是对话多阶段图表示学习算法（DialogMSG）。 引入从不同对话范围建模的多阶段图以捕获更有效的信息。 另一个是双约束模块。 该模块不仅包括一个话语级分类器，还包括一个对话级图分类器，命名为 Atmosphere。 大量实验的结果表明，所提出的方法优于 IEMOCAP 基准数据集上的当前技术水平。</t>
+  </si>
+  <si>
+    <t>发现卷积神经网络 (CNN) 在学习语音情感识别的表示方面非常有效。 CNN 没有明确地模拟光谱/时间/通道轴中特征的关联或相对重要性。 在本文中，我们提出了一个名为 spectro-temporal-channel (STC) 注意模块的注意模块，它与 CNN 集成以提高表示学习能力。 我们的模块沿时间、频率和 CNN 通道这三个维度推断出注意力图。 在IEMOCAP数据库上进行了实验，以评估所提出的表示学习方法的有效性。 结果表明，所提出的方法在 F1 分数方面比传统的 CNN 方法有 3.13% 的绝对增长。</t>
+  </si>
+  <si>
+    <t>虽然语音情感识别 (SER) 已得到积极研究，但与语音识别和说话人识别任务相比，训练数据的数量和变化是有限的。 因此，结合多个语料库来训练广义 SER 模型是有希望的。 然而，情绪表达的方式因环境、任务领域和语言而异。 特别是，行为数据集和自发数据集之间存在不匹配，因为前者包含比后者更丰富和明确的情感表达。 在本文中，我们研究了基于多任务学习（MTL）并考虑风格属性的有效组合方法。 我们还假设样本数量最多的中性表达不受风格的影响，因此提出了一种选择性 MTL 方法，将 MTL 应用于除中性类别之外的情感类别。 使用 IEMOCAP 数据库和呼叫中心数据集进行的实验评估证实了两个语料库、MTL 和建议的选择性 MTL 组合的效果。</t>
+  </si>
+  <si>
+    <t>深度学习研究领域极大地受益于自我监督学习。 在此范例中，任务独立模型使用大量未标记数据进行预训练，任务特定模型在自监督模型上进行训练。 语音处理中的大多数自我监督技术分为三类。 在第一类中，使用了不同的架构和建设性的 InfoNCE 损失[6、7、8、9、10]。 第二类是基于掩码标记分类 [11]。 第三类采用重建损失，使用各种技术，例如生成未来帧 [12、13] 和编码器-解码器方法来重建输入的屏蔽部分 [14、15、16]。 深度神经网络擅长拟合训练集。 因此，他们倾向于大量利用数据特征和标签之间的表面相关性。 虽然这可以提高训练集的性能，但可能会损害模型的泛化能力。 为了克服这个问题，提出了多种方法来消除模型学习不良线索的能力。 纳格拉尼等人。 [17] 建议使用“混淆损失”，这是通过将预测与均匀分布进行比较来计算的交叉熵损失。 加宁等。 [18] 使用关于数据域的额外知识来解决域适应问题。 他们建议通过否定预测域标签的损失梯度来归一化域特征。 与那些方法相反，我们根据任务而不是领域对线索进行标准化。 此外，我们的方法侧重于自监督表示框架。 语音情绪识别基于话语预测情绪。 最广泛使用的语音情感识别基准是交互式情感二元运动捕捉数据库（IEMOCAP）[3]。 为了语音情感识别，早期的端到端方法结合了卷积神经网络 (CNN) 和长短期记忆 (LSTM) [19,20,21]。 后来，基于注意力的模型优于 CNN 和 LSTM 组合，因为它们能够专注于输入的特定部分 [22、23、24]。 近年来，由于自监督学习模型能够从未标记的数据中学习高质量的表示，因此在语音处理研究中引起了极大的兴趣。 反映这一点，杨等人。 [25] 在他们的基准测试中证明，自我监督模型在情绪识别方面产生了最先进的结果。 我们提出了一种通过将自监督模型与说话人特征归一化相结合来增强语音情感识别的方法。</t>
+  </si>
+  <si>
+    <t>大型语音情感识别数据集很难获得，小型数据集可能包含偏差。 反过来，基于深度网络的分类器很容易利用这些偏差并找到说话者特征等捷径。 这些捷径通常会损害模型的泛化能力。 为了应对这一挑战，我们提出了一种基于梯度的对抗学习框架，该框架可以学习语音情感识别任务，同时从特征表示中归一化说话人的特征。 我们展示了我们的方法在与说话者无关和与说话者相关的设置上的有效性，并在具有挑战性的 IEMOCAP 数据集上获得了最新的最新结果。</t>
+  </si>
+  <si>
+    <t>语音是人与人沟通的主要媒介，在每个人的日常生活中都扮演着重要的角色。 语音情感识别（SER）旨在预测语音中反映的情感。 SER 是各种智能应用程序的一项基本任务。 例如，SER 通过更好地理解用户的意图和状态，为智能机器人带来更好的用户体验。 因此，研究团体对 SER 任务的兴趣增加了 [1]。 最近，受到计算机视觉令人振奋的进步的启发，现有研究 [2、3、4、5、6、7、8、9] 通过将光谱特征视为图像，在 SER 上取得了很大的改进。 标准的卷积神经网络 (CNN) 架构主要由特征表示和注意力图组成。 通常，特征表示通常学习固定尺度的特征来捕获所有信息特征。 此外，注意力图用于关注局部固定尺度特征中的大多数情感信息[6、7、8、9]。 然而，情绪的特点是发音随时间变化的光谱特征具有不同尺度的变化。 由于 SER 中现有 CNN 的局限性，我们提出了一种新颖的 GLobal-Aware 多尺度 (GLAM) 神经网络。 在我们的工作中，由于情绪中的时间跨度和语调强度不同，我们利用多尺度卷积块来提取不同尺度的特征。 此外，引入了全局感知融合模块来选择反映不同尺度情绪模式的重要信息。 实验表明，与最先进的 CNN 模型相比，多尺度特征表示和全局感知融合都可以带来很大的改进[9]。 我们的贡献可以总结如下： • 据我们所知，我们是第一个将多尺度特征表示应用于 SER 的人。 此外，这种表示还极大地增强了现有的 CNN。 • 我们引入了一个新的全局感知融合模块来获取跨多个尺度的情感信息。 我们的研究显示了不同粒度之间信息融合的巨大潜力。 • 实验证明了我们提出的模型在 SER 的四个常用指标上的优越性。 与最先进的方法相比，我们在 IEMOCAP 语料库上实现了 2.5% 到 4.5% 的改进。 本文的其余部分安排如下。 我们在第 2 节中回顾了相关方法。第 3 节介绍了所提出的 GLAM 神经网络。 最后，第 4 节和第 5 节是实验结果和结论。 方法被用来学习特征表示以预测每个特征段的情感标签[10]。 然后，通过将特征片段视为图像，卷积网络显示出对 SER [2、4、6、8、9、11、12] 特征表示的巨大影响。 最后，极限学习机 (ELM) [10]、胶囊网络 [12] 和 LSTM [2、11] 等各种方法已被应用于融合来自所有特征段的所有特征表示。 然而，大多数现有的 CNN 专注于固定尺度的局部特征而忽略了变化尺度的影响，这在我们提出的模型中得到了充分考虑。 最近，基于注意力的模型在 SER [6,7,8,9,13] 上取得了重大进展。 例如，多头注意力图通过卷积运算学习，根据周围信息选择重要信息[8]。 此外，进一步引入区域注意力来计算不同卷积范围的重要性[9]。 尽管局部信息对于描述细微信息很有用，但缺乏感知全局信息限制了现有基于注意力的方法的进步。 因此，我们提出了一个全局感知融合模块来计算全局注意力图并融合不同尺度的情感信息。</t>
+  </si>
+  <si>
+    <t>语音情感识别 (SER) 是一项从语音数据中预测情感标签的基本任务。 最近的工作主要集中在使用卷积神经网络 (CNN) 通过将时变光谱特征视为图像来学习固定尺度特征表示上的局部注意力图。 然而，由于现有 CNN 对 SER 的限制，无法很好地捕获不同尺度的丰富情感特征和重要的全局信息。 在本文中，我们提出了一种新颖的 GLobal-Aware Multi-scale (GLAM) 神经网络 1，通过全局感知融合模块学习多尺度特征表示来处理情感信息。 具体来说，GLAM 迭代地利用具有不同尺度的多个卷积核来学习多个特征表示。 然后，不使用基于注意力的方法，而是应用一个简单但有效的全局感知融合模块来获取全局最重要的情感信息。 在基准语料库 IEMOCAP 上对四种情绪进行的实验证明了我们提出的模型的优越性，与以前的最先进方法相比，四种常用指标提高了 2.5% 到 4.5%。</t>
+  </si>
+  <si>
+    <t>我们研究了时间上下文对于语音情感识别 (SER) 的重要性。 开发了两个分别在传统特征和学习特征上训练的 SER 系统来预测情绪的分类标签。 对于传统的声学特征，我们研究了滤波器组特征和韵律特征的组合，以及当这些特征的时间上下文通过可学习的光谱时间感受野 (STRF) 扩展时对 SER 的影响。 实验表明，在可学习的 STRF 上训练的系统优于使用类似设置评估的其他报告系统。 我们还证明了使用长时间上下文进行预训练的 wav2vec 特征优于传统特征。 然后，我们引入了一个新的基于片段的学习目标来约束我们的分类器从大的时间上下文中提取局部情绪特征。 结合学习目标和微调策略，我们使用 wav2vec 特征的顶线系统在 IEMOCAP 数据集上达到了最先进的性能。</t>
+  </si>
+  <si>
+    <t>随着人工智能的不断发展，情感计算领域越来越受到研究者的关注。 情感识别是情感计算的重要组成部分，旨在从收集到的人脸、语音和文本数据中识别出有意义的信息。 在这些数据中，语音是情感信息的重要来源，它不仅包含交际内容，还包含情感等副语言信息。 近年来，语音情感识别（SER）在人工客服[1]、远程教育[2]和医学[3]等诸多领域得到了广泛的应用。 然而，由于某些特定情绪之间的严重混淆，识别语音中表达的情绪仍然具有挑战性。 特征提取是 SER 系统中的一个重要过程，旨在为不同的情绪产生有效的特征表示。 在 SER 的声学特征提取方面，基于低级描述符 (LLD) 和高级统计泛函 (HSF) [4, 5, 6] 的几个特征集，包括 INTERSPEECH-2010 [7]，GeMAPS [8]、AVEC2013 [9] 和 ComParE [10] 已被开发用于广泛的应用。 随着计算能力的提高，深度学习方法成为主流，为高级特征捕获提供了卓越的能力。 例如，Han 等人。 [11] 使用深度神经网络 (DNN) 提取 MFCC 和音调的片段级特征，其中包含情感上有效的信息。 毛等。 [12] 首先采用卷积神经网络 (CNN) 从 SER 的频谱图中学习空间特征，并在一些基准数据集上表现出出色的性能。 李等。 [13] 使用递归神经网络 (RNN) 来解释情绪言语中的长上下文效应。 陈等。 [14] 使用 LSTM 学习 SER 的长期依赖性和上下文信息。 然而，大多数先前研究中的一个共同问题是特征混淆，即来自不同情感类别的聚类可能相互重叠 [15]。 为了解决这个问题，Huang 等人。 [16] 利用 hard-positive 挖掘技术来评估三元组损失的性能。 刘等人。 [17] 通过选择硬三元组提出了一个使用三元组损失的 SER 框架，以更好地区分情感分类中的混淆。 高等。 [18] 引入了度量学习来衡量三元组输入的相似性，并鼓励模型为 SER 提取更具辨别力的特征。 然而，所有以前的方法都从根据当前网络很难的训练样本中挖掘出困难三元组，从而使经过训练的特征嵌入网络容易受到不良局部最优的影响 [19, 20]。 在本文中，我们引入了一种对抗性联合损失策略来明确地激发所学特征之间的类内紧凑性和类间可分离性，其中应用生成器和鉴别器来生成对全局优化网络非常重要的硬三元组。 SER 的另一个关键问题是如何有效地突出与情感相关的区域，因为语音中的特征对情感识别的贡献不均。 受视觉分析 [21, 22] 成功的启发，研究人员引入了时空注意力来提高 SER 系统的性能 [23, 24]。 李等。 [15] 提出了时空注意力来提取频率特征。 然而，时空注意力突出了不同特征对 SER 的贡献，而忽略了语音中的时间特征。 刘等人。 [25] 引入了自我注意机制，它捕获了时间特征的长期依赖性，并允许模型专注于情感显着特征。 因此，我们提出了将时空注意力与自我注意力相结合的级联注意力，以定位一些目标情绪区域并捕获长距离依赖。 本文的主要贡献总结如下：（1）我们提出了一个级联注意力网络（CAN）来提取有效的情感特征，其中时空注意力定位一些目标情感区域，自注意力可以补偿长距离依赖 . (2) 我们引入了一种对抗性联合损失策略来区分不同类别的相似情感嵌入，其中生成器和鉴别器用于生成硬三元组以全局优化网络，而不是仅探索当前网络的现有样本。 (3) 在基准数据集 IEMOCAP 上的实验结果表明，我们的方法在 WA 和 UA 中分别达到了 76.17% 和 72.95%。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>语音情感识别（SER）是一项旨在理解语音中潜在情感信息的任务。 近年来，人们对 SER 的兴趣激增，因为情感在人机交互过程中传达了至关重要的信息。 然而，通常有两个障碍阻碍了 SER 的应用：SER 数据集的不平衡和稀缺性问题。 我们可以从两个角度进一步描述问题。 首先，SER 数据集有一个共同的问题，即不同情感类别之间的语音数据分布不均匀或高度倾斜。 标记为“中性”的话语比标记为“快乐、愤怒等”的话语更频繁。 各种情绪类别的数据稀缺导致数据集高度不平衡。 为了缓解数据不平衡问题，一种常见的方法是通过数据增强技术生成合成数据。 [1] 中的作者使用香草生成对抗网络 (GAN) [2] 生成合成 openSMILE 声学特征 [3] 用于 SER 任务的训练。 在 [4] 中，作者使用 CycleGAN [5] 将 openSMILE 特征向量从一个情感类别转移到另一个情感类别。 一些方法不使用 openSMILE 功能，而是对低级声学功能（例如 Mel-Spectrogram）进行增强，这对于其他任务来说是一个优势。 [6、7] 中的方法应用 starGAN [8] 将中性情绪的语音表达转换为其他情绪。 [9] 中的作者修改了 GAN 以对不平衡数据进行扩充，他们凭经验证明该 GAN 可以提高不平衡数据集下的 SER 性能。 考虑稀缺性问题的另一个重要方面是各种现有口语的数据可用性。 许多语言可用的数据资源非常少，这对这些语言的SER研究和应用构成了重大障碍。 解决此问题的一种方法是在一种或多种语言上使用足够的数据（源）训练 SER 模型，并结合其他语言的极少训练话语（目标）。 这个想法是利用从源语言中获得的知识来提高低资源目标语言的性能[10]。 这种跨越不同语言的 SER 训练策略，即跨语言 SER，已被广泛研究 [11,12,13]。 尽管添加源语言提高了目标语言的 SER 性能，但跨语言 SER 任务仍有改进的空间。 在本文中，我们提出了一种增强策略，可用于解决数据不平衡和稀缺问题。 我们增强方法的一个组成部分是 GAN，其生成器用于增强。 生成器的灵感来自 [14]，其中作者成功地为多个下游任务执行了自动增强。 为了稳定 GAN 或提高其性能，通常在训练期间引入额外的辅助目标 [15、16、17]。 因此，我们应用基于三元组损失的表征学习器来从原始数据中学习情绪表征。 表示学习器的学习知识用于增加和稳定 SER 任务的增强性能。 我们将我们的贡献总结如下：1）我们为 SER 任务提出了基于 GAN 的增强。 2) 我们证明我们的扩充方法可以在高度不平衡的数据集下大大提高 SER 性能（我们的扩充召回率 +8%）。 3) 此外，对于跨语言 SER 任务，我们的扩充提高了三种不同目标语言的性能，只有大约 50 个话语。</t>
-  </si>
-  <si>
-    <t>语音情感识别 (SER) 对于人机交互至关重要，但由于两个主要障碍仍然是一个具有挑战性的问题：数据稀缺和不平衡。 许多 SER 数据集基本上是不平衡的，其中一类（通常是中性）的数据话语比其他类的数据话语更频繁。 此外，只有少数数据资源可用于许多现有的口头语言。 为了解决这些问题，我们利用由三元组网络引导的基于 GAN 的增强模型，以在训练数据不平衡和不足的情况下提高 SER 性能。 我们进行实验并证明：1）在高度不平衡的数据集下，我们的增强策略显着提高了 SER 性能（与基线相比 +8% 的召回率）。 2) 此外，在跨语言基准测试中，我们训练了一个具有足够源语言话语但目标语言话语很少（在我们的实验中大约 50 个）的模型，我们的增强策略为所有三种目标语言的 SER 性能带来了好处。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>随着自动语音识别（Automatic Speech Recognition，ASR）的快速发展，语音识别领域被视为一个有前途的研究领域。 特别是，语音情感识别（SER）是刑事侦查、医疗、实时情感分析等最关键的技术之一。在移动设备上的实时情感识别等轻量级 SER 应用中，模型具有 仅语音模态比更重的多模态（文本和语音）模型更可取。 我们的目标是提高此类任务的 SER 准确性。 适用于 SER 的特征集已在 INTERSPEECH 2009 (IS09) 情感挑战赛 [1]、AVEC 挑战赛 [2] 和扩展的日内瓦简约声学参数集 (eGeMAPS) [3] 中得到研究和使用。 这些功能集通常是手工制作的低级描述符 (LLD)。 然而，由于深度学习模型的发展，最近的研究 [4、5、6、7] 有效地使用了直接从幅度相关特征（例如频谱图或梅尔频率倒谱系数 (MFCC)）中提取的任务特定特征。 根据最近的研究，我们将 MFCC 用于我们的端到端方法。 尽管深度学习方法提供了良好的性能，但由于它们提供的是黑盒模型，因此结果难以理解或解释。 减轻缺点的一种方法是使用注意力机制。 从推理过程中提取的注意力图有助于理解整个特征空间的注意力分布。 此外，注意力机制可以通过更多地关注特征空间的关键区域来提高性能。 由于可以通过注意力分布直观地分析图像和文本，因此已经进行了许多计算机视觉和自然语言处理 [8, 9, 10, 11] 的研究，以通过更多地关注关键区域和调整错位来提高注意力性能。 然而，语音信号中的关键区域不像图像或文本那样直观，因此难以理解和分析注意力图。 在 SER 中，[12] 表明最高振幅在情绪识别性能中起着重要作用，因为每种情绪都有不同的分贝水平。 基于这项研究，我们假设检测最大振幅并学习相关表示可以提高情绪识别性能。 在实验中，我们通过可视化注意力图并显示基于注意力对齐调整的性能改进来评估假设。 我们首先探讨多头自注意力 [13]，语音识别中最常用的注意力机制之一，是否检测到 SER 中的关键区域（最高振幅）。 在探索中，我们通过现有多头自注意力中注意力图的可视化来识别注意力和振幅之间的偏差。 为了减轻注意力图的错位并提高性能，在本文中，我们提出了一种焦点-注意力（FA）机制和一种新颖的校准-注意力（CA）机制。 文档摘要任务 [14] 中使用的 FA 机制采用高斯分布来关注具有显着信息的区域。 在这项工作中，FA 起着检测片段中最大幅度部分的作用。 由于 multi-head self-attention 存在多个 attention alignments，并不是所有的 attention heads 都有合适的 alignment。 我们提出了新的 CA 机制，通过为每个注意力头分配不同的权重来调节信息流，并提高周围上下文的利用率。 在实验中，我们使用 IEMOCAP [15] 和 RAVDESS [16] 数据集，它们是流行的 SER 基准数据集，我们证明我们的方法实现了最先进的结果。 然后我们将所提出的方法的注意力图可视化，并证明调整错位可以提高 SER 性能。 我们的贡献如下： • 我们在 SER 中应用焦点-注意机制来检测片段中最大幅度的部分。 • 我们提出了一种新颖的校准-注意机制来调节信息流并提高周围环境的利用率。 • 在实验中，我们在IEMOCAP 和RAVDESS 数据集上实现了最先进的性能，并显着改进了现有最先进的方法。</t>
-  </si>
-  <si>
-    <t>深度学习架构的最新发展促使我们使用频谱图或音频功能（例如 MFCC），而不是手工制作的 LLD。 [6] 直接从语音频谱图中提取特征，而不是使用传统的手工制作的特征来更好地表示情感。 这些提取的特征用作卷积神经网络 (CNN) 的输入。 [7] 将 Mel 频谱图和 MFCC 用于包含两个独立神经网络的双层模型。 他们通过提取两个具有不同窗口大小的不同 Mel 频谱图来解决时频权衡问题。 此外，他们还通过实验表明，梅尔频谱图比 MFCC 更难学习。 我们目前的工作使用 MFCC。 目前，几乎所有的深度学习应用都在使用注意力机制。 注意机制可以通过更多地关注特征空间的关键区域来提高性能。 注意力还可以在一定程度上缓解黑盒问题，这是深度学习模型结构的一个缺点。 在语音识别领域，注意力机制已被用于 ASR [17, 18] 和 SER [19, 20, 21] 等任务。 特别是，在 [13] 在机器翻译任务中表现出强大的自注意力之后，自注意力也试图在 SER 任务 [6, 22] 中为关键区域分配更多权重，并证明了其有效性。 [6] 使用自我注意机制来关注出现在特定部分而不是整个话语中的情绪。 [22] 结合扩张残差网络 (DRN) 和多头自注意力来增强情绪显着信息的导入，我们在本文中将该模型表示为 DRN-MHSA。 SER 中其他最先进的模型如下。 Audio-BRE [23] 使用基于使用 MFCC 的长短期记忆 (LSTM) 的双向循环编码器 (BRE) 模型。 A-DCNN [24] 使用 SincNet 过滤器层 [25] 从语音音频中学习自定义过滤器组。 与 [6, 22] 使用现有的自注意力不同，我们提出了使用 FA 和 CA 机制改进的自注意力，并验证了检测最大振幅和学习表达表示可以提高情绪识别性能的假设。</t>
-  </si>
-  <si>
-    <t>注意力已经成为深度学习方法中最常用的机制之一。 注意机制可以帮助系统更多地关注特征空间的关键区域。 例如，高振幅区域可以在语音情感识别 (SER) 中发挥重要作用。 在本文中，我们确定了现有多头自注意力中注意力与信号幅度之间的错位。 为了改善注意力区域，我们建议结合多头自注意力使用焦点-注意力 (FA) 机制和新颖的校准-注意力 (CA) 机制。 通过FA机制，网络可以检测出片段中最大幅度的部分。 通过采用 CA 机制，网络可以通过为每个注意力头分配不同的权重来调节信息流，并提高周围上下文的利用率。 为了评估所提出的方法，使用 IEMOCAP 和 RAVDESS 数据集进行了实验。 实验结果表明，所提出的框架在两个数据集上都明显优于最先进的方法。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>情绪是影响人类目的表达、意图理解和决策制定的重要内部状态[1]。 为了提供有效的服务，一些公司采用语音情感识别技术来跟踪客户的感受 [2]。 人机交互领域的其他研究人员开发了情绪检测系统来改善用户体验 [3]。 近几十年来，特征工程 [4, 5] 和深度学习模型 [6, 7] 的发展极大地改善了语音情感识别。 由于语音样本具有时间序列属性，许多研究采用门控循环单元 (GRU) [8]、长短期记忆网络 (LSTM) [9]，或卷积神经网络 (CNN) 和 LSTM 的组合 [ 10] 感知时间序列信息。 除了考虑语音中包含的特征序列外，还提出了可以分析对话中上下文信息的新模型。 叶等人。 [8] 提出了一个交互感知网络来考虑对话中的上下文。 焦等。 [11] 通过考虑上下文构建了用于话语级情绪识别的分层门控循环单元。 上述研究在上下文信息的帮助下显着提高了语音情感识别的性能。 为了捕捉对标签分配最有贡献的情感框架，研究人员采用了注意力机制 [12]，还借鉴了多实例学习的思想来识别和关注语音话语中最显着的部分 [13]。 此外，由于言语中的情感因素因性别和人而异，Latif 等人。 [14]提出了一种多任务学习框架来提高语音情感识别的性能。 尽管在语音情感识别领域取得了进展，但很少有研究探讨数据正则化的好处。 众所周知，说话人的语音情感表达是不同的，这种偏差可能会给同一类别下的样本形成聚类或具有不规则边界（非高斯分布）的样本带来困难。 这种情况可能会使模型容易在域内数据集上过度拟合，对模式分布的局部不规则性敏感，跨域实现的分数也会降低 [15,16,17]。 为了通过正则化潜在表示的分布来平滑边界并赋予模型专注于最显着的语音片段的能力，在本研究中，我们提出了一种具有多实例学习的基于对抗性自动编码器的分类器。 我们提出的模型中的鉴别器可以将潜在表示映射到高维高斯分布。 我们还采用了具有性别和情绪分类的多任务学习策略。 所提出的模型在 IEMOCAP [18] 数据集上进行了训练，并在语料库 (IEMOCAP) 和跨语料库验证集 (MELD [19]) 上进行了评估。 我们的论文结构如下。 我们在第 2 节中描述了我们提出的方法的细节。实验设置和结果在第 3 节中描述。讨论在第 4 节中介绍，第 5 节简要总结了我们的工作。</t>
-  </si>
-  <si>
-    <t>在本文中，我们提出了一种基于对抗性自动编码器的分类器，它可以规范潜在表示的分布以平滑类别之间的边界。 此外，我们采用多实例学习，将语音分成多个片段，以捕捉表达情绪的最显着时刻。 所提出的模型在 IEMOCAP 数据集上进行了训练，并在语料库验证集 (IEMOCAP) 和跨语料库验证集 (MELD) 上进行了评估。 实验结果表明，我们的模型优于语料库内验证的基线，并通过正则化提高了跨语料库验证的分数。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>语音情感识别（SER）越来越受到研究者的关注，因为它不仅在人机交互方面具有巨大的应用前景，而且在智能认知助手[1]、在线教育[2]等领域的应用也越来越广泛 ]、电脑游戏[3]等。 近年来，一些深度学习方法如深度神经网络（DNNs）[4]、卷积神经网络（CNNs）[5]、递归神经网络（RNNs）[6, 7]和注意力机制[8, 9] 已用于 SER 任务并取得了有竞争力的结果。 特别是，Satt 等人。 [10] 提出 CNN-BLSTM 方法是一项经典工作，它首先引入 CNN 来提取特征，然后采用双向长短期记忆网络 (BLSTM) [11] 来学习话语内上下文信息。 尽管目前的研究取得了不错的成果，但在实际应用中将其部署到对话场景中仍然存在差距。 最近，一些自然语言处理（NLP）工作尝试更进一步，例如 DialogueRNN [12]。 该方法引入了具有注意机制的 RNN，以从未来和过去最相关的文本中学习话语间信息。 然而，远程上下文建模的性能受制于 RNN 的结构。 另一项代表性工作是引入图卷积神经网络（GCN）[13]，例如 DialogueGCN [14] 和 RGAT [15]。 这两项工作都引入了 GCN 来捕获一次对话中的话语关系，并在 NLP 中取得了竞争性的结果。 由于GCNs中存在的过度平滑问题，卷积层的数量不能灵活应对不同的范围。 同时，上述方法只是对一个句子进行建模，缺乏对整个当前对话的考虑。 为了解决上述问题，我们提出了一种新颖的对话级上下文信息学习系统，如图 1 所示。首先，我们引入 CNN-BLSTM 从频谱图中提取话语级表示。 其次，将学习到的话语级表示转换为对话级格式。 以下对话级策略由两个模块组成。 在第一个模块中，对话多阶段图表示学习算法 (DialogMSG) 被提出来捕获每个对话中的上下文依赖性。 在图构建中，对话中的话语被表示为节点，话语之间的依赖关系被视为边。 考虑到序列建模，未来的信息不应该泄露给过去。 采用基于单向门循环单元 (GRU) [16] 的局部更新机制来表示过去的上下文信息。 为了进一步捕获远程上下文信息，还引入了一种集成残差连接的多阶段结构。基于残差多阶段GRU的图结构确保即使在远程对话中也能有效保留关键信息。 而且DialogueGCN中过平滑的问题也能得到很好的缓解。 在第二个模块中，设置了一个对话中每个话语的传统分类约束。 同时，还考虑了对对话图分类的约束，命名为Atmosphere。 总之，我们的贡献如下： • DialogMSG 被提议通过残差多阶段基于 GRU 的图来捕获从局部区域到全局区域的上下文信息。 • 首次考虑了名为Atmosphere 的约束，以获得对远程对话中情绪变化的更高敏感度。</t>
-  </si>
-  <si>
-    <t>随着语音情感识别（SER）的发展，目前的研究大多是话语级的，不能适应实际场景的需要。 在本文中，我们提出了一种新颖的策略，专注于捕获对话级别的上下文信息。 基于卷积神经网络 (CNN) 和双向长短期记忆网络 (BLSTM) 学习的话语级表示，所提出的对话级方法由两个模块组成。 第一个模块是对话多阶段图表示学习算法（DialogMSG）。 引入从不同对话范围建模的多阶段图以捕获更有效的信息。 另一个是双约束模块。 该模块不仅包括一个话语级分类器，还包括一个对话级图分类器，命名为 Atmosphere。 大量实验的结果表明，所提出的方法优于 IEMOCAP 基准数据集上的当前技术水平。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>情感识别在人机交互中起着至关重要的作用，可以提高用户体验水平，提供良好的交互性[1]。 随着人机交互的快速发展，语音情感识别（SER）越来越受到研究人员的关注。 然而，学习 SER 的有效表示仍然是一个挑战 [2]。 典型的情绪识别模型包括两个步骤。 他们首先选择基于听觉的特征（如音调、能量等），然后构建分类器来区分情绪 [3]。 例如，Luengo 等人。 [4] 采用支持向量机 (SVM) 作为分类器来区分情绪。 随着深度学习的出现，Wang 等人。 [5] 使用深度神经网络 (DNN) 从基于听觉的特征中学习高级表示，然后训练极限学习机 (ELM) 作为分类器。 萧等人。 [6] 提出将注意力机制集成到 SER 的深度递归神经网络模型中。 近年来，提出了一些基于卷积神经网络（CNN）的模型来提取深度表示[7-10]。 在这些研究中，基于 CNN 的方法因其丰富的表示能力而成为最常用的方法之一 [11]。 人们认为情绪信息体现在频谱域和时间域中 [12, 13]。 在时间域中，情绪反映在不同的时间范围内（即，讲话与沉默）。 此外，音素携带不同的情感信息。 在频谱域中，一些情绪（例如愤怒）在较高频率下表现出丰富的声学特征，而一些情绪（例如悲伤）在低频下表现出丰富的声学特征。 在 [12] 中，设计了两组不同形状的滤波器来从输入频谱图中捕获频谱和时间信息。 [14] 为 SER 采用了时频 CNN (TFCNN)。 TFCNN 使用 CNN 分别提取时间感知和频率感知表示。 这些表示是从每个维度单独学习的。 他们没有明确地模拟特征在光谱/时间轴上的相对重要性。 此外，他们没有考虑通道域，而每个通道中的特征图具有不同的重要性[15]。 受先前研究的启发，我们提出了一种具有光谱时间通道 (STC) 注意力的表示学习方法，如图 1 所示，该方法同时考虑了时间、光谱和通道维度。 我们的目标是通过使用可以与任何 CNN 集成的 STC 注意模块来增强表示能力。 该模块明确包括沿光谱时间 (ST) 和通道维度的注意机制。 ST 注意力集中在情感信息时间帧和频率点上，通道注意力集中在判别特征图上并去除冗余。 拟议的 3D STC 注意力图可以学习关注“什么”和“哪里”。</t>
-  </si>
-  <si>
-    <t>发现卷积神经网络 (CNN) 在学习语音情感识别的表示方面非常有效。 CNN 没有明确地模拟光谱/时间/通道轴中特征的关联或相对重要性。 在本文中，我们提出了一个名为 spectro-temporal-channel (STC) 注意模块的注意模块，它与 CNN 集成以提高表示学习能力。 我们的模块沿时间、频率和 CNN 通道这三个维度推断出注意力图。 在IEMOCAP数据库上进行了实验，以评估所提出的表示学习方法的有效性。 结果表明，所提出的方法在 F1 分数方面比传统的 CNN 方法有 3.13% 的绝对增长。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>最近，基于语音的交互系统已经部署在许多设备中，例如智能手机、智能扬声器和社交机器人，但是情感识别的功能和能力仍然有限。 语音情感识别 (SER) 有很大的改进空间 [1, 2]。 虽然与 SER 相关的设置和任务领域多种多样，但由于收集数据的便利性，大多数传统研究都集中在行为情绪数据集上 [3, 4, 5]。 心理学领域的研究表明，自发的情绪表达与行为的情绪表达之间存在很大差距 [6, 7]。 这里，表演的情绪表达包括给定场景表达的情绪表达（例如IEMOCAP [8]数据库和电影数据集，如AFEW [9]），而自发的情绪表达是指在现实生活中表达的情绪表达。 显然，与后者相比，前者的表达方式更为丰富和明确。 对真正的自发 SER 的研究数量有限。 在 [10] 中，基于高斯混合模型 (GMM) 的分类器使用了 3 个不同的特征，但 3 类情绪分类（积极、消极和中性）的结果仅略好于随机基线。 最近，[11] 表明结合先验知识和分类器融合提高了 SER 在自发语音中的性能，[12] 提出了一种用于自发语音的多尺度深度卷积 LSTM。 另一方面，最近针对行动数据集的 SER 研究给出了许多新的想法和模型来提高性能。 在 [13] 中，针对 SER 任务提出了一种基于注意力池的卷积神经网络 (CNN)。 [14] 和 [15] 都表明双向 LSTM（Bi-LSTM）多头自注意力模型可以为 SER 带来很大的提升。 [16] 和 [17] 表明，向 SER 模型添加文本特征也可以带来显着的改进。 然而，在现实世界的嘈杂环境中自动转录自发的和情绪化的语音并不容易，大的单词错误率会对 SER 性能产生负面影响。 因此，在本研究中，我们不使用任何文本级特征，而是专注于基于音频的特征。 当我们关注基于音频的特征时，很容易组合多个数据集，而不管任务领域和训练通用模型的语言。 在这项研究中，我们探索了一个行为数据集和一个自发数据集的组合，以提高这两个数据集的 SER 性能。 它将缓解 SER 任务中数据稀疏性的瓶颈，这与自动语音识别任务相比更为严重。 在这种情况下，我们需要考虑到 SER 模型中情感表达风格的差异。 一个简单的解决方案是使用多任务学习 (MTL)。 李等。 [18] 尝试使用 MTL 进行语言和性别识别，但没有表现出改善。 另一方面，李等人。 [15] 在 IEMOCAP 数据库中展示了 MTL 与性别识别的效果，因为性别之间的情绪表达是不同的。 在这项工作中，我们研究了具有风格识别的 MTL，其中风格要么是表演的，要么是自发的。 此外，我们假设中性情绪的表达是普遍的并且独立于风格和数据集。 因此，我们还提出了一种新的选择性 MTL 方法，将 MTL 应用于中性类别以外的情感类别。 我们在第 2 节中描述了我们的基线模型和建议的模型，并在第 3 节中介绍了我们在本研究中使用的两个语料库。第 4 节详细介绍了实验设置、结果和分析。 最后，第 5 节给出了结论。</t>
-  </si>
-  <si>
-    <t>虽然语音情感识别 (SER) 已得到积极研究，但与语音识别和说话人识别任务相比，训练数据的数量和变化是有限的。 因此，结合多个语料库来训练广义 SER 模型是有希望的。 然而，情绪表达的方式因环境、任务领域和语言而异。 特别是，行为数据集和自发数据集之间存在不匹配，因为前者包含比后者更丰富和明确的情感表达。 在本文中，我们研究了基于多任务学习（MTL）并考虑风格属性的有效组合方法。 我们还假设样本数量最多的中性表达不受风格的影响，因此提出了一种选择性 MTL 方法，将 MTL 应用于除中性类别之外的情感类别。 使用 IEMOCAP 数据库和呼叫中心数据集进行的实验评估证实了两个语料库、MTL 和建议的选择性 MTL 组合的效果。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>在过去十年中，语音处理方面的进步令人印象深刻。 个人语音助理之类的挑战在十年前还令人望而生畏，如今已成为我们日常工作的一部分。 这些系统的一个关键部分是与用户交互并了解他的意图和情绪。 了解用户的情绪可以在用户和系统之间建立信任，改善用户体验。 因此，提高语音情感识别的准确性成为近年来的主要研究热点。 报告的改进在很大程度上是由于大型通用和特定任务数据集的可用性 [1, 2]、计算性能的进步（例如，对于 GPU）以及更好地理解如何将归纳偏差编码为深度 神经网络。 自监督学习方法的使用在文本和视觉模态的进步中发挥了至关重要的作用，因为它们能够从未标记的数据中学习强大的特征表示。 最近，这些技术在语音处理领域也取得了成功。 语音情感识别的注释具有挑战性，因为它受到注释者对语言、文化和社会约束的偏见的影响。 特别是语音情感识别会在说话者特征和录音的情感类别之间产生有偏差的虚假相关性。 多年来已经创建了多个数据集，用于训练和评估用于语音情感识别的机器学习方法 [3、4、5]。 他们中的大多数都比较小。 从有偏见的小数据集学习的困难是深度学习研究社区面临的主要挑战。 经典的自监督学习过程依赖于在大型未标记数据集上训练的表征，以及在相对较小的标记数据集上训练的下游任务。 通常，我们的方法通过使用标签与下游任务标签不同的第三个数据集来提高下游任务的性能。 例如，在这项工作中，对于说话人的情绪识别，我们的方法从自监督表示中归一化不需要的特征，以提高语音情绪识别任务的性能。 我们通过学习一种特征表示来实现这一点，该特征表示在语音情感识别方面表现出色，同时对说话人的特征足够稳健（见图 1）。 我们提出的方法在说话者相关和说话者无关设置方面优于当前最先进的结果。 总之，我们提出了一个从自我监督表示中进行说话人特征归一化的通用框架。 我们解决了小数据集设置问题，并在 IEMOCAP 基准上为其提出了一个框架。 通过广泛的实验，我们表明我们的方法在几个设置上优于当前的语音情感识别最先进的结果。 其余工作组织如下： 图 2 概述了相关工作。 秒。 3描述了我们提出的方法。 秒。 4报告了我们方法的实验和结果。 最后，秒。 5 总结论文。</t>
-  </si>
-  <si>
-    <t>深度学习研究领域极大地受益于自我监督学习。 在此范例中，任务独立模型使用大量未标记数据进行预训练，任务特定模型在自监督模型上进行训练。 语音处理中的大多数自我监督技术分为三类。 在第一类中，使用了不同的架构和建设性的 InfoNCE 损失[6、7、8、9、10]。 第二类是基于掩码标记分类 [11]。 第三类采用重建损失，使用各种技术，例如生成未来帧 [12、13] 和编码器-解码器方法来重建输入的屏蔽部分 [14、15、16]。 深度神经网络擅长拟合训练集。 因此，他们倾向于大量利用数据特征和标签之间的表面相关性。 虽然这可以提高训练集的性能，但可能会损害模型的泛化能力。 为了克服这个问题，提出了多种方法来消除模型学习不良线索的能力。 纳格拉尼等人。 [17] 建议使用“混淆损失”，这是通过将预测与均匀分布进行比较来计算的交叉熵损失。 加宁等。 [18] 使用关于数据域的额外知识来解决域适应问题。 他们建议通过否定预测域标签的损失梯度来归一化域特征。 与那些方法相反，我们根据任务而不是领域对线索进行标准化。 此外，我们的方法侧重于自监督表示框架。 语音情绪识别基于话语预测情绪。 最广泛使用的语音情感识别基准是交互式情感二元运动捕捉数据库（IEMOCAP）[3]。 为了语音情感识别，早期的端到端方法结合了卷积神经网络 (CNN) 和长短期记忆 (LSTM) [19,20,21]。 后来，基于注意力的模型优于 CNN 和 LSTM 组合，因为它们能够专注于输入的特定部分 [22、23、24]。 近年来，由于自监督学习模型能够从未标记的数据中学习高质量的表示，因此在语音处理研究中引起了极大的兴趣。 反映这一点，杨等人。 [25] 在他们的基准测试中证明，自我监督模型在情绪识别方面产生了最先进的结果。 我们提出了一种通过将自监督模型与说话人特征归一化相结合来增强语音情感识别的方法。</t>
-  </si>
-  <si>
-    <t>大型语音情感识别数据集很难获得，小型数据集可能包含偏差。 反过来，基于深度网络的分类器很容易利用这些偏差并找到说话者特征等捷径。 这些捷径通常会损害模型的泛化能力。 为了应对这一挑战，我们提出了一种基于梯度的对抗学习框架，该框架可以学习语音情感识别任务，同时从特征表示中归一化说话人的特征。 我们展示了我们的方法在与说话者无关和与说话者相关的设置上的有效性，并在具有挑战性的 IEMOCAP 数据集上获得了最新的最新结果。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>语音是人与人沟通的主要媒介，在每个人的日常生活中都扮演着重要的角色。 语音情感识别（SER）旨在预测语音中反映的情感。 SER 是各种智能应用程序的一项基本任务。 例如，SER 通过更好地理解用户的意图和状态，为智能机器人带来更好的用户体验。 因此，研究团体对 SER 任务的兴趣增加了 [1]。 最近，受到计算机视觉令人振奋的进步的启发，现有研究 [2、3、4、5、6、7、8、9] 通过将光谱特征视为图像，在 SER 上取得了很大的改进。 标准的卷积神经网络 (CNN) 架构主要由特征表示和注意力图组成。 通常，特征表示通常学习固定尺度的特征来捕获所有信息特征。 此外，注意力图用于关注局部固定尺度特征中的大多数情感信息[6、7、8、9]。 然而，情绪的特点是发音随时间变化的光谱特征具有不同尺度的变化。 由于 SER 中现有 CNN 的局限性，我们提出了一种新颖的 GLobal-Aware 多尺度 (GLAM) 神经网络。 在我们的工作中，由于情绪中的时间跨度和语调强度不同，我们利用多尺度卷积块来提取不同尺度的特征。 此外，引入了全局感知融合模块来选择反映不同尺度情绪模式的重要信息。 实验表明，与最先进的 CNN 模型相比，多尺度特征表示和全局感知融合都可以带来很大的改进[9]。 我们的贡献可以总结如下： • 据我们所知，我们是第一个将多尺度特征表示应用于 SER 的人。 此外，这种表示还极大地增强了现有的 CNN。 • 我们引入了一个新的全局感知融合模块来获取跨多个尺度的情感信息。 我们的研究显示了不同粒度之间信息融合的巨大潜力。 • 实验证明了我们提出的模型在 SER 的四个常用指标上的优越性。 与最先进的方法相比，我们在 IEMOCAP 语料库上实现了 2.5% 到 4.5% 的改进。 本文的其余部分安排如下。 我们在第 2 节中回顾了相关方法。第 3 节介绍了所提出的 GLAM 神经网络。 最后，第 4 节和第 5 节是实验结果和结论。</t>
-  </si>
-  <si>
-    <t>语音是人与人沟通的主要媒介，在每个人的日常生活中都扮演着重要的角色。 语音情感识别（SER）旨在预测语音中反映的情感。 SER 是各种智能应用程序的一项基本任务。 例如，SER 通过更好地理解用户的意图和状态，为智能机器人带来更好的用户体验。 因此，研究团体对 SER 任务的兴趣增加了 [1]。 最近，受到计算机视觉令人振奋的进步的启发，现有研究 [2、3、4、5、6、7、8、9] 通过将光谱特征视为图像，在 SER 上取得了很大的改进。 标准的卷积神经网络 (CNN) 架构主要由特征表示和注意力图组成。 通常，特征表示通常学习固定尺度的特征来捕获所有信息特征。 此外，注意力图用于关注局部固定尺度特征中的大多数情感信息[6、7、8、9]。 然而，情绪的特点是发音随时间变化的光谱特征具有不同尺度的变化。 由于 SER 中现有 CNN 的局限性，我们提出了一种新颖的 GLobal-Aware 多尺度 (GLAM) 神经网络。 在我们的工作中，由于情绪中的时间跨度和语调强度不同，我们利用多尺度卷积块来提取不同尺度的特征。 此外，引入了全局感知融合模块来选择反映不同尺度情绪模式的重要信息。 实验表明，与最先进的 CNN 模型相比，多尺度特征表示和全局感知融合都可以带来很大的改进[9]。 我们的贡献可以总结如下： • 据我们所知，我们是第一个将多尺度特征表示应用于 SER 的人。 此外，这种表示还极大地增强了现有的 CNN。 • 我们引入了一个新的全局感知融合模块来获取跨多个尺度的情感信息。 我们的研究显示了不同粒度之间信息融合的巨大潜力。 • 实验证明了我们提出的模型在 SER 的四个常用指标上的优越性。 与最先进的方法相比，我们在 IEMOCAP 语料库上实现了 2.5% 到 4.5% 的改进。 本文的其余部分安排如下。 我们在第 2 节中回顾了相关方法。第 3 节介绍了所提出的 GLAM 神经网络。 最后，第 4 节和第 5 节是实验结果和结论。 方法被用来学习特征表示以预测每个特征段的情感标签[10]。 然后，通过将特征片段视为图像，卷积网络显示出对 SER [2、4、6、8、9、11、12] 特征表示的巨大影响。 最后，极限学习机 (ELM) [10]、胶囊网络 [12] 和 LSTM [2、11] 等各种方法已被应用于融合来自所有特征段的所有特征表示。 然而，大多数现有的 CNN 专注于固定尺度的局部特征而忽略了变化尺度的影响，这在我们提出的模型中得到了充分考虑。 最近，基于注意力的模型在 SER [6,7,8,9,13] 上取得了重大进展。 例如，多头注意力图通过卷积运算学习，根据周围信息选择重要信息[8]。 此外，进一步引入区域注意力来计算不同卷积范围的重要性[9]。 尽管局部信息对于描述细微信息很有用，但缺乏感知全局信息限制了现有基于注意力的方法的进步。 因此，我们提出了一个全局感知融合模块来计算全局注意力图并融合不同尺度的情感信息。</t>
-  </si>
-  <si>
-    <t>语音情感识别 (SER) 是一项从语音数据中预测情感标签的基本任务。 最近的工作主要集中在使用卷积神经网络 (CNN) 通过将时变光谱特征视为图像来学习固定尺度特征表示上的局部注意力图。 然而，由于现有 CNN 对 SER 的限制，无法很好地捕获不同尺度的丰富情感特征和重要的全局信息。 在本文中，我们提出了一种新颖的 GLobal-Aware Multi-scale (GLAM) 神经网络 1，通过全局感知融合模块学习多尺度特征表示来处理情感信息。 具体来说，GLAM 迭代地利用具有不同尺度的多个卷积核来学习多个特征表示。 然后，不使用基于注意力的方法，而是应用一个简单但有效的全局感知融合模块来获取全局最重要的情感信息。 在基准语料库 IEMOCAP 上对四种情绪进行的实验证明了我们提出的模型的优越性，与以前的最先进方法相比，四种常用指标提高了 2.5% 到 4.5%。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>近年来，自动语音情感识别（SER）受到越来越多的关注。 研究表明，可以使用帧级声学特征以及从更大的时间跨度计算的副语言学特征来实现情绪识别 [1, 2]。 在本文中，我们专注于创建一个准确的情绪分类器，该分类器结合使用相关的声学线索和正确的时间跨度来整合提取的特征。 已经为 SER 探索了各种基于知识和学习的特征。 其中许多方法都基于短时谱特征（例如 [3]、[4] 等）。 还探索了中期调制特征 [5] 和韵律特征 [6、7]。 除了个体特征外，还发现各种形式和分辨率的特征组合有助于预测效价和唤醒 [8] 或分类情绪 [4]。 以无监督方式在大规模语料库上训练的学习特征为上述特征提供了一种有吸引力的替代方案。 Wav2vec [9] 是此类学习特征的一个示例，因为它从原始波形计算跨越长时间上下文窗口的特征。 尽管它在自动语音识别 (ASR) 和说话人识别任务中取得了成功，但只有少数研究 [10、11] 探索了将此功能用于 SER。 博涅等人。 [11] 表明 wav2vec 在 SER 上的表现优于低级描述符和频谱图。 马卡里等人。 [10] 发现 wav2vec 和 BERTlike [12] 特征的联合使用在连续 SER 任务上优于 word2vec [13] 的短时倒谱特征。 这些研究表明，从 wav2vec 中学习到的表征对 SER 是有益的。 除了使用在不同时间跨度上提取的特征外，上下文感知分类器的使用一直是 SER 的一种流行方法。 虽然许多研究依赖于 DNN 架构（例如长短期记忆 (LSTM)）从长期上下文中隐式学习，但使此类过程明确且目标更明确已证明是有益的。 Aldeneh 等人。 [14] 通过改变卷积神经网络 (CNN) 的过滤器大小来明确地模拟他们系统的上下文跨度（作者称为“区域显着性”）。 相比之下，一些作品 [3、15、16] 发现执行帧级分类并使用简单的平均 [3] 或在提取的帧级特征 [15、16] 之上训练另一个分类器以产生 话语级预测。 虽然还没有关于为话语级决策聚合帧级决策的最佳方法的主导理论，但这些方法表明这两种方法对 SER 都是有用的。 在本文中，我们研究了几个 SER 特征以及扩展这些特征的时间上下文的效果。 我们分别基于声学特征和学习特征开发了两个系统。 对于声学特征，我们选择了跨越不同级别声学背景的三个代表性特征。 使用我们已经证明可以区分语音质量的受限 CNN 自动提取调制特征 [17]。 对于学习到的特征，我们专注于 wav2vec [9]，它跨越比传统特征更长的时间上下文。 然而，长时间的上下文往往包含过多的信息，并使分类器容易受到虚假相关的影响。 受 SER [3、15、16] 现有基于分段的分类器的启发，我们设计了一个新的训练目标，它限制学习的表示以从每个学习的特征帧预测情绪。 将此目标与 wav2vec 的微调策略相结合，我们的系统在 IEMOCAP 数据集上优于以前的方法。 本文的组织。 在下一节中，我们将介绍我们的语音情感识别方法。 然后我们描述评估程序。 最后，我们讨论我们的实验结果。</t>
-  </si>
-  <si>
-    <t>我们研究了时间上下文对于语音情感识别 (SER) 的重要性。 开发了两个分别在传统特征和学习特征上训练的 SER 系统来预测情绪的分类标签。 对于传统的声学特征，我们研究了滤波器组特征和韵律特征的组合，以及当这些特征的时间上下文通过可学习的光谱时间感受野 (STRF) 扩展时对 SER 的影响。 实验表明，在可学习的 STRF 上训练的系统优于使用类似设置评估的其他报告系统。 我们还证明了使用长时间上下文进行预训练的 wav2vec 特征优于传统特征。 然后，我们引入了一个新的基于片段的学习目标来约束我们的分类器从大的时间上下文中提取局部情绪特征。 结合学习目标和微调策略，我们使用 wav2vec 特征的顶线系统在 IEMOCAP 数据集上达到了最先进的性能。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -857,16 +867,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F04CE1E-A7B7-4F3E-963C-C989CEAA1B0A}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G19" sqref="F2:G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="5.5546875" style="1" customWidth="1"/>
-    <col min="3" max="4" width="11.77734375" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="5.5546875" style="1" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="11.77734375" style="1" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="0" style="1" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="69.5546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="49.88671875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -889,10 +902,10 @@
         <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -915,10 +928,10 @@
         <v>78</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>24</v>
+        <v>79</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>79</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -941,10 +954,10 @@
         <v>80</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -964,13 +977,13 @@
         <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>84</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -990,13 +1003,13 @@
         <v>34</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1016,13 +1029,13 @@
         <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H6" s="1" t="s">
-        <v>88</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1042,13 +1055,13 @@
         <v>39</v>
       </c>
       <c r="F7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H7" s="1" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1068,13 +1081,13 @@
         <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>92</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1094,13 +1107,13 @@
         <v>43</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>94</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1120,13 +1133,13 @@
         <v>46</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>24</v>
+        <v>95</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1146,13 +1159,13 @@
         <v>48</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -1172,13 +1185,13 @@
         <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>102</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1198,13 +1211,13 @@
         <v>54</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>24</v>
+        <v>99</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>104</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1244,13 +1257,13 @@
         <v>57</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>24</v>
+        <v>100</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>106</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1270,13 +1283,13 @@
         <v>59</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>24</v>
+        <v>101</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>108</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1296,13 +1309,13 @@
         <v>62</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1322,13 +1335,13 @@
         <v>65</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1348,17 +1361,17 @@
         <v>68</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>24</v>
+        <v>106</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>116</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G20" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
vault backup: 2023-01-28 17:32:13
</commit_message>
<xml_diff>
--- a/emotion/3.论文记录/语音情感识别-摘要-引言摘录.xlsx
+++ b/emotion/3.论文记录/语音情感识别-摘要-引言摘录.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\mypack\人生规划\3.进修\2.升学\04.硕士学习\3.研究\笔记\emotion\3.论文记录\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8B87F69F-EDD1-480B-A2F1-64D68D88E461}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788FA903-3FE8-40A1-96D3-AFBFAB61226C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="216" windowWidth="12204" windowHeight="9816" xr2:uid="{51BD2796-7EA4-47CC-B162-5BC723D3BEC4}"/>
+    <workbookView xWindow="-5376" yWindow="6804" windowWidth="12204" windowHeight="9816" xr2:uid="{51BD2796-7EA4-47CC-B162-5BC723D3BEC4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -542,7 +541,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -551,6 +550,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -867,8 +869,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F04CE1E-A7B7-4F3E-963C-C989CEAA1B0A}">
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G19" sqref="F2:G19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -877,7 +879,7 @@
     <col min="2" max="2" width="5.5546875" style="1" hidden="1" customWidth="1"/>
     <col min="3" max="4" width="11.77734375" style="1" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="69.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="69.5546875" style="4" customWidth="1"/>
     <col min="7" max="7" width="49.88671875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -898,7 +900,7 @@
       <c r="E1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -908,7 +910,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="358.8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>30</v>
       </c>
@@ -924,7 +926,7 @@
       <c r="E2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>78</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -934,7 +936,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>25</v>
       </c>
@@ -950,7 +952,7 @@
       <c r="E3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>80</v>
       </c>
       <c r="G3" s="1" t="s">
@@ -960,7 +962,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -976,7 +978,7 @@
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>107</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -986,7 +988,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -1002,7 +1004,7 @@
       <c r="E5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>84</v>
       </c>
       <c r="G5" s="1" t="s">
@@ -1012,7 +1014,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="400.2" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>36</v>
       </c>
@@ -1028,7 +1030,7 @@
       <c r="E6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="4" t="s">
         <v>86</v>
       </c>
       <c r="G6" s="1" t="s">
@@ -1038,7 +1040,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -1054,7 +1056,7 @@
       <c r="E7" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="4" t="s">
         <v>88</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -1064,7 +1066,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
@@ -1080,7 +1082,7 @@
       <c r="E8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="4" t="s">
         <v>90</v>
       </c>
       <c r="G8" s="1" t="s">
@@ -1090,7 +1092,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="262.2" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1106,7 +1108,7 @@
       <c r="E9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="4" t="s">
         <v>92</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1116,7 +1118,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
@@ -1132,7 +1134,7 @@
       <c r="E10" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="4" t="s">
         <v>108</v>
       </c>
       <c r="G10" s="1" t="s">
@@ -1142,7 +1144,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
@@ -1158,7 +1160,7 @@
       <c r="E11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="4" t="s">
         <v>109</v>
       </c>
       <c r="G11" s="1" t="s">
@@ -1168,7 +1170,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="358.8" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>51</v>
       </c>
@@ -1184,7 +1186,7 @@
       <c r="E12" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="4" t="s">
         <v>110</v>
       </c>
       <c r="G12" s="1" t="s">
@@ -1194,7 +1196,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
@@ -1210,7 +1212,7 @@
       <c r="E13" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="4" t="s">
         <v>111</v>
       </c>
       <c r="G13" s="1" t="s">
@@ -1230,7 +1232,7 @@
       <c r="D14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G14" s="1" t="s">
@@ -1240,7 +1242,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="345" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>56</v>
       </c>
@@ -1256,7 +1258,7 @@
       <c r="E15" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="4" t="s">
         <v>112</v>
       </c>
       <c r="G15" s="1" t="s">
@@ -1266,7 +1268,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1282,7 +1284,7 @@
       <c r="E16" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="4" t="s">
         <v>113</v>
       </c>
       <c r="G16" s="1" t="s">
@@ -1292,7 +1294,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="358.8" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>61</v>
       </c>
@@ -1308,7 +1310,7 @@
       <c r="E17" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="4" t="s">
         <v>114</v>
       </c>
       <c r="G17" s="1" t="s">
@@ -1318,7 +1320,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="303.60000000000002" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
@@ -1334,7 +1336,7 @@
       <c r="E18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="4" t="s">
         <v>115</v>
       </c>
       <c r="G18" s="1" t="s">
@@ -1344,7 +1346,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>67</v>
       </c>
@@ -1360,7 +1362,7 @@
       <c r="E19" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="4" t="s">
         <v>116</v>
       </c>
       <c r="G19" s="1" t="s">
@@ -1391,7 +1393,7 @@
       <c r="E21" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G21" s="1" t="s">
@@ -1417,7 +1419,7 @@
       <c r="E22" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -1443,7 +1445,7 @@
       <c r="E23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="F23" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G23" s="1" t="s">
@@ -1469,7 +1471,7 @@
       <c r="E24" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="F24" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G24" s="1" t="s">
@@ -1495,7 +1497,7 @@
       <c r="E25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="F25" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G25" s="1" t="s">
@@ -1521,7 +1523,7 @@
       <c r="E26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="1" t="s">
+      <c r="F26" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G26" s="1" t="s">
@@ -1547,7 +1549,7 @@
       <c r="E27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="F27" s="4" t="s">
         <v>24</v>
       </c>
       <c r="G27" s="1" t="s">
@@ -1560,6 +1562,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="180" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>